<commit_message>
Deploying to gh-pages from  @ 90bcaf012f05dc57052050351a5729e716050e26 🚀
</commit_message>
<xml_diff>
--- a/assets/excel/2022_2-3-4.xlsx
+++ b/assets/excel/2022_2-3-4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Hannover\Dez15-Uebergreifende-Analysen\Projekte\Integrationsmonitoring\github\MT_Site\assets\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{49918677-1824-4284-8961-2A656B0B7CB5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E3FD296-6A78-4DCD-BEA3-E624EE584862}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14010" xr2:uid="{2C0D3989-42FD-490A-A21B-E034F5A30F90}"/>
   </bookViews>
@@ -356,22 +356,10 @@
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -415,6 +403,18 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -734,9 +734,7 @@
   <sheetPr codeName="Tabelle1"/>
   <dimension ref="B1:R48"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:B8"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -759,1684 +757,1684 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="2:18" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="3" t="s">
+    <row r="6" spans="2:18" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
-      <c r="L6" s="4"/>
-      <c r="M6" s="4"/>
-      <c r="N6" s="4"/>
-      <c r="O6" s="4"/>
-      <c r="P6" s="4"/>
-      <c r="Q6" s="4"/>
-      <c r="R6" s="4"/>
-    </row>
-    <row r="7" spans="2:18" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="6"/>
-      <c r="C7" s="7">
+      <c r="C6" s="22"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="22"/>
+      <c r="G6" s="22"/>
+      <c r="H6" s="22"/>
+      <c r="I6" s="22"/>
+      <c r="J6" s="22"/>
+      <c r="K6" s="22"/>
+      <c r="L6" s="22"/>
+      <c r="M6" s="22"/>
+      <c r="N6" s="22"/>
+      <c r="O6" s="22"/>
+      <c r="P6" s="22"/>
+      <c r="Q6" s="22"/>
+      <c r="R6" s="22"/>
+    </row>
+    <row r="7" spans="2:18" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="20"/>
+      <c r="C7" s="4">
         <v>2006</v>
       </c>
-      <c r="D7" s="7">
+      <c r="D7" s="4">
         <v>2007</v>
       </c>
-      <c r="E7" s="7">
+      <c r="E7" s="4">
         <v>2008</v>
       </c>
-      <c r="F7" s="7">
+      <c r="F7" s="4">
         <v>2009</v>
       </c>
-      <c r="G7" s="7">
+      <c r="G7" s="4">
         <v>2010</v>
       </c>
-      <c r="H7" s="7">
+      <c r="H7" s="4">
         <v>2011</v>
       </c>
-      <c r="I7" s="7">
+      <c r="I7" s="4">
         <v>2012</v>
       </c>
-      <c r="J7" s="7">
+      <c r="J7" s="4">
         <v>2013</v>
       </c>
-      <c r="K7" s="7">
+      <c r="K7" s="4">
         <v>2014</v>
       </c>
-      <c r="L7" s="7">
+      <c r="L7" s="4">
         <v>2015</v>
       </c>
-      <c r="M7" s="7">
+      <c r="M7" s="4">
         <v>2016</v>
       </c>
-      <c r="N7" s="7">
+      <c r="N7" s="4">
         <v>2017</v>
       </c>
-      <c r="O7" s="7">
+      <c r="O7" s="4">
         <v>2018</v>
       </c>
-      <c r="P7" s="7">
+      <c r="P7" s="4">
         <v>2019</v>
       </c>
-      <c r="Q7" s="7">
+      <c r="Q7" s="4">
         <v>2020</v>
       </c>
-      <c r="R7" s="7">
+      <c r="R7" s="4">
         <v>2021</v>
       </c>
     </row>
-    <row r="8" spans="2:18" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="8"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
-      <c r="J8" s="4"/>
-      <c r="K8" s="4"/>
-      <c r="L8" s="4"/>
-      <c r="M8" s="4"/>
-      <c r="N8" s="4"/>
-      <c r="O8" s="4"/>
-      <c r="P8" s="4"/>
-      <c r="Q8" s="4"/>
-      <c r="R8" s="4"/>
-    </row>
-    <row r="9" spans="2:18" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="2:18" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25">
-      <c r="B10" s="9" t="s">
+    <row r="8" spans="2:18" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="21"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="22"/>
+      <c r="E8" s="22"/>
+      <c r="F8" s="22"/>
+      <c r="G8" s="22"/>
+      <c r="H8" s="22"/>
+      <c r="I8" s="22"/>
+      <c r="J8" s="22"/>
+      <c r="K8" s="22"/>
+      <c r="L8" s="22"/>
+      <c r="M8" s="22"/>
+      <c r="N8" s="22"/>
+      <c r="O8" s="22"/>
+      <c r="P8" s="22"/>
+      <c r="Q8" s="22"/>
+      <c r="R8" s="22"/>
+    </row>
+    <row r="9" spans="2:18" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="2:18" s="6" customFormat="1" ht="8.25" x14ac:dyDescent="0.25">
+      <c r="B10" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="10">
+      <c r="C10" s="6">
         <v>7567</v>
       </c>
-      <c r="D10" s="10">
+      <c r="D10" s="6">
         <v>5866</v>
       </c>
-      <c r="E10" s="10">
+      <c r="E10" s="6">
         <v>4488</v>
       </c>
-      <c r="F10" s="10">
+      <c r="F10" s="6">
         <v>3947</v>
       </c>
-      <c r="G10" s="10">
+      <c r="G10" s="6">
         <v>4205</v>
       </c>
-      <c r="H10" s="10">
+      <c r="H10" s="6">
         <v>4595</v>
       </c>
-      <c r="I10" s="10">
+      <c r="I10" s="6">
         <v>5096</v>
       </c>
-      <c r="J10" s="10">
+      <c r="J10" s="6">
         <v>4900</v>
       </c>
-      <c r="K10" s="10">
+      <c r="K10" s="6">
         <v>4399</v>
       </c>
-      <c r="L10" s="10">
+      <c r="L10" s="6">
         <v>4598</v>
       </c>
-      <c r="M10" s="10">
+      <c r="M10" s="6">
         <v>4880</v>
       </c>
-      <c r="N10" s="10">
+      <c r="N10" s="6">
         <v>5044</v>
       </c>
-      <c r="O10" s="10">
+      <c r="O10" s="6">
         <v>4743</v>
       </c>
-      <c r="P10" s="10">
+      <c r="P10" s="6">
         <v>6722</v>
       </c>
-      <c r="Q10" s="10">
+      <c r="Q10" s="6">
         <v>4041</v>
       </c>
-      <c r="R10" s="10">
+      <c r="R10" s="6">
         <v>4066</v>
       </c>
     </row>
-    <row r="11" spans="2:18" s="12" customFormat="1" ht="8.25" x14ac:dyDescent="0.25">
-      <c r="B11" s="11" t="s">
+    <row r="11" spans="2:18" s="8" customFormat="1" ht="8.25" x14ac:dyDescent="0.25">
+      <c r="B11" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="12">
+      <c r="C11" s="8">
         <v>35</v>
       </c>
-      <c r="D11" s="12">
+      <c r="D11" s="8">
         <v>33</v>
       </c>
-      <c r="E11" s="12">
+      <c r="E11" s="8">
         <v>58</v>
       </c>
-      <c r="F11" s="12">
+      <c r="F11" s="8">
         <v>60</v>
       </c>
-      <c r="G11" s="12">
+      <c r="G11" s="8">
         <v>92</v>
       </c>
-      <c r="H11" s="12">
+      <c r="H11" s="8">
         <v>62</v>
       </c>
-      <c r="I11" s="12">
+      <c r="I11" s="8">
         <v>61</v>
       </c>
-      <c r="J11" s="12">
+      <c r="J11" s="8">
         <v>70</v>
       </c>
-      <c r="K11" s="12">
+      <c r="K11" s="8">
         <v>68</v>
       </c>
-      <c r="L11" s="12">
+      <c r="L11" s="8">
         <v>73</v>
       </c>
-      <c r="M11" s="12">
+      <c r="M11" s="8">
         <v>76</v>
       </c>
-      <c r="N11" s="12">
+      <c r="N11" s="8">
         <v>100</v>
       </c>
-      <c r="O11" s="12">
+      <c r="O11" s="8">
         <v>92</v>
       </c>
-      <c r="P11" s="12">
+      <c r="P11" s="8">
         <v>85</v>
       </c>
-      <c r="Q11" s="12">
+      <c r="Q11" s="8">
         <v>114</v>
       </c>
-      <c r="R11" s="12">
+      <c r="R11" s="8">
         <v>124</v>
       </c>
     </row>
-    <row r="12" spans="2:18" s="12" customFormat="1" ht="8.25" x14ac:dyDescent="0.25">
-      <c r="B12" s="11" t="s">
+    <row r="12" spans="2:18" s="8" customFormat="1" ht="8.25" x14ac:dyDescent="0.25">
+      <c r="B12" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C12" s="12">
+      <c r="C12" s="8">
         <v>96</v>
       </c>
-      <c r="D12" s="12">
+      <c r="D12" s="8">
         <v>109</v>
       </c>
-      <c r="E12" s="12">
+      <c r="E12" s="8">
         <v>98</v>
       </c>
-      <c r="F12" s="12">
+      <c r="F12" s="8">
         <v>69</v>
       </c>
-      <c r="G12" s="12">
+      <c r="G12" s="8">
         <v>72</v>
       </c>
-      <c r="H12" s="12">
+      <c r="H12" s="8">
         <v>126</v>
       </c>
-      <c r="I12" s="12">
+      <c r="I12" s="8">
         <v>344</v>
       </c>
-      <c r="J12" s="12">
+      <c r="J12" s="8">
         <v>231</v>
       </c>
-      <c r="K12" s="12">
+      <c r="K12" s="8">
         <v>195</v>
       </c>
-      <c r="L12" s="12">
+      <c r="L12" s="8">
         <v>191</v>
       </c>
-      <c r="M12" s="12">
+      <c r="M12" s="8">
         <v>222</v>
       </c>
-      <c r="N12" s="12">
+      <c r="N12" s="8">
         <v>224</v>
       </c>
-      <c r="O12" s="12">
+      <c r="O12" s="8">
         <v>206</v>
       </c>
-      <c r="P12" s="12">
+      <c r="P12" s="8">
         <v>157</v>
       </c>
-      <c r="Q12" s="12">
+      <c r="Q12" s="8">
         <v>127</v>
       </c>
-      <c r="R12" s="12">
+      <c r="R12" s="8">
         <v>195</v>
       </c>
     </row>
-    <row r="13" spans="2:18" s="12" customFormat="1" ht="8.25" x14ac:dyDescent="0.25">
-      <c r="B13" s="11" t="s">
+    <row r="13" spans="2:18" s="8" customFormat="1" ht="8.25" x14ac:dyDescent="0.25">
+      <c r="B13" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="13">
+      <c r="C13" s="9">
         <v>85</v>
       </c>
-      <c r="D13" s="13">
+      <c r="D13" s="9">
         <v>70</v>
       </c>
-      <c r="E13" s="13">
+      <c r="E13" s="9">
         <v>88</v>
       </c>
-      <c r="F13" s="13">
+      <c r="F13" s="9">
         <v>53</v>
       </c>
-      <c r="G13" s="12">
+      <c r="G13" s="8">
         <v>52</v>
       </c>
-      <c r="H13" s="12">
+      <c r="H13" s="8">
         <v>77</v>
       </c>
-      <c r="I13" s="12">
+      <c r="I13" s="8">
         <v>89</v>
       </c>
-      <c r="J13" s="12">
+      <c r="J13" s="8">
         <v>114</v>
       </c>
-      <c r="K13" s="12">
+      <c r="K13" s="8">
         <v>128</v>
       </c>
-      <c r="L13" s="12">
+      <c r="L13" s="8">
         <v>139</v>
       </c>
-      <c r="M13" s="12">
+      <c r="M13" s="8">
         <v>160</v>
       </c>
-      <c r="N13" s="12">
+      <c r="N13" s="8">
         <v>226</v>
       </c>
-      <c r="O13" s="12">
+      <c r="O13" s="8">
         <v>199</v>
       </c>
-      <c r="P13" s="12">
+      <c r="P13" s="8">
         <v>170</v>
       </c>
-      <c r="Q13" s="12">
+      <c r="Q13" s="8">
         <v>153</v>
       </c>
-      <c r="R13" s="12">
+      <c r="R13" s="8">
         <v>214</v>
       </c>
     </row>
-    <row r="14" spans="2:18" s="12" customFormat="1" ht="8.25" x14ac:dyDescent="0.25">
-      <c r="B14" s="11" t="s">
+    <row r="14" spans="2:18" s="8" customFormat="1" ht="8.25" x14ac:dyDescent="0.25">
+      <c r="B14" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C14" s="13" t="s">
+      <c r="C14" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="D14" s="13" t="s">
+      <c r="D14" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="E14" s="13" t="s">
+      <c r="E14" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="F14" s="12">
+      <c r="F14" s="8">
         <v>34</v>
       </c>
-      <c r="G14" s="12">
+      <c r="G14" s="8">
         <v>170</v>
       </c>
-      <c r="H14" s="12">
+      <c r="H14" s="8">
         <v>221</v>
       </c>
-      <c r="I14" s="12">
+      <c r="I14" s="8">
         <v>181</v>
       </c>
-      <c r="J14" s="12">
+      <c r="J14" s="8">
         <v>222</v>
       </c>
-      <c r="K14" s="12">
+      <c r="K14" s="8">
         <v>216</v>
       </c>
-      <c r="L14" s="12">
+      <c r="L14" s="8">
         <v>242</v>
       </c>
-      <c r="M14" s="12">
+      <c r="M14" s="8">
         <v>215</v>
       </c>
-      <c r="N14" s="12">
+      <c r="N14" s="8">
         <v>247</v>
       </c>
-      <c r="O14" s="12">
+      <c r="O14" s="8">
         <v>217</v>
       </c>
-      <c r="P14" s="12">
+      <c r="P14" s="8">
         <v>188</v>
       </c>
-      <c r="Q14" s="12">
+      <c r="Q14" s="8">
         <v>171</v>
       </c>
-      <c r="R14" s="12">
+      <c r="R14" s="8">
         <v>175</v>
       </c>
     </row>
-    <row r="15" spans="2:18" s="12" customFormat="1" ht="8.25" x14ac:dyDescent="0.25">
-      <c r="B15" s="11" t="s">
+    <row r="15" spans="2:18" s="8" customFormat="1" ht="8.25" x14ac:dyDescent="0.25">
+      <c r="B15" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C15" s="12">
+      <c r="C15" s="8">
         <v>864</v>
       </c>
-      <c r="D15" s="12">
+      <c r="D15" s="8">
         <v>583</v>
       </c>
-      <c r="E15" s="12">
+      <c r="E15" s="8">
         <v>548</v>
       </c>
-      <c r="F15" s="12">
+      <c r="F15" s="8">
         <v>434</v>
       </c>
-      <c r="G15" s="12">
+      <c r="G15" s="8">
         <v>422</v>
       </c>
-      <c r="H15" s="12">
+      <c r="H15" s="8">
         <v>477</v>
       </c>
-      <c r="I15" s="12">
+      <c r="I15" s="8">
         <v>518</v>
       </c>
-      <c r="J15" s="12">
+      <c r="J15" s="8">
         <v>655</v>
       </c>
-      <c r="K15" s="12">
+      <c r="K15" s="8">
         <v>576</v>
       </c>
-      <c r="L15" s="12">
+      <c r="L15" s="8">
         <v>559</v>
       </c>
-      <c r="M15" s="12">
+      <c r="M15" s="8">
         <v>650</v>
       </c>
-      <c r="N15" s="12">
+      <c r="N15" s="8">
         <v>664</v>
       </c>
-      <c r="O15" s="12">
+      <c r="O15" s="8">
         <v>598</v>
       </c>
-      <c r="P15" s="12">
+      <c r="P15" s="8">
         <v>644</v>
       </c>
-      <c r="Q15" s="12">
+      <c r="Q15" s="8">
         <v>572</v>
       </c>
-      <c r="R15" s="12">
+      <c r="R15" s="8">
         <v>619</v>
       </c>
     </row>
-    <row r="16" spans="2:18" s="12" customFormat="1" ht="8.25" x14ac:dyDescent="0.25">
-      <c r="B16" s="11" t="s">
+    <row r="16" spans="2:18" s="8" customFormat="1" ht="8.25" x14ac:dyDescent="0.25">
+      <c r="B16" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C16" s="12">
+      <c r="C16" s="8">
         <v>90</v>
       </c>
-      <c r="D16" s="12">
+      <c r="D16" s="8">
         <v>209</v>
       </c>
-      <c r="E16" s="12">
+      <c r="E16" s="8">
         <v>124</v>
       </c>
-      <c r="F16" s="12">
+      <c r="F16" s="8">
         <v>119</v>
       </c>
-      <c r="G16" s="12">
+      <c r="G16" s="8">
         <v>136</v>
       </c>
-      <c r="H16" s="12">
+      <c r="H16" s="8">
         <v>132</v>
       </c>
-      <c r="I16" s="12">
+      <c r="I16" s="8">
         <v>81</v>
       </c>
-      <c r="J16" s="12">
+      <c r="J16" s="8">
         <v>115</v>
       </c>
-      <c r="K16" s="12">
+      <c r="K16" s="8">
         <v>113</v>
       </c>
-      <c r="L16" s="12">
+      <c r="L16" s="8">
         <v>156</v>
       </c>
-      <c r="M16" s="12">
+      <c r="M16" s="8">
         <v>193</v>
       </c>
-      <c r="N16" s="12">
+      <c r="N16" s="8">
         <v>241</v>
       </c>
-      <c r="O16" s="12">
+      <c r="O16" s="8">
         <v>239</v>
       </c>
-      <c r="P16" s="12">
+      <c r="P16" s="8">
         <v>337</v>
       </c>
-      <c r="Q16" s="12">
+      <c r="Q16" s="8">
         <v>369</v>
       </c>
-      <c r="R16" s="12">
+      <c r="R16" s="8">
         <v>369</v>
       </c>
     </row>
-    <row r="17" spans="2:18" s="12" customFormat="1" ht="8.25" x14ac:dyDescent="0.25">
-      <c r="B17" s="11" t="s">
+    <row r="17" spans="2:18" s="8" customFormat="1" ht="8.25" x14ac:dyDescent="0.25">
+      <c r="B17" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C17" s="12">
+      <c r="C17" s="8">
         <v>475</v>
       </c>
-      <c r="D17" s="12">
+      <c r="D17" s="8">
         <v>405</v>
       </c>
-      <c r="E17" s="12">
+      <c r="E17" s="8">
         <v>188</v>
       </c>
-      <c r="F17" s="12">
+      <c r="F17" s="8">
         <v>257</v>
       </c>
-      <c r="G17" s="12">
+      <c r="G17" s="8">
         <v>304</v>
       </c>
-      <c r="H17" s="12">
+      <c r="H17" s="8">
         <v>283</v>
       </c>
-      <c r="I17" s="12">
+      <c r="I17" s="8">
         <v>299</v>
       </c>
-      <c r="J17" s="12">
+      <c r="J17" s="8">
         <v>245</v>
       </c>
-      <c r="K17" s="12">
+      <c r="K17" s="8">
         <v>251</v>
       </c>
-      <c r="L17" s="12">
+      <c r="L17" s="8">
         <v>168</v>
       </c>
-      <c r="M17" s="12">
+      <c r="M17" s="8">
         <v>225</v>
       </c>
-      <c r="N17" s="12">
+      <c r="N17" s="8">
         <v>157</v>
       </c>
-      <c r="O17" s="12">
+      <c r="O17" s="8">
         <v>132</v>
       </c>
-      <c r="P17" s="12">
+      <c r="P17" s="8">
         <v>149</v>
       </c>
-      <c r="Q17" s="12">
+      <c r="Q17" s="8">
         <v>131</v>
       </c>
-      <c r="R17" s="12">
+      <c r="R17" s="8">
         <v>117</v>
       </c>
     </row>
-    <row r="18" spans="2:18" s="12" customFormat="1" ht="9" x14ac:dyDescent="0.25">
-      <c r="B18" s="11" t="s">
+    <row r="18" spans="2:18" s="8" customFormat="1" ht="9" x14ac:dyDescent="0.25">
+      <c r="B18" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C18" s="12">
+      <c r="C18" s="8">
         <v>1800</v>
       </c>
-      <c r="D18" s="12">
+      <c r="D18" s="8">
         <v>1198</v>
       </c>
-      <c r="E18" s="12">
+      <c r="E18" s="8">
         <v>540</v>
       </c>
-      <c r="F18" s="12">
+      <c r="F18" s="8">
         <v>109</v>
       </c>
-      <c r="G18" s="12">
+      <c r="G18" s="8">
         <v>187</v>
       </c>
-      <c r="H18" s="12">
+      <c r="H18" s="8">
         <v>258</v>
       </c>
-      <c r="I18" s="12">
+      <c r="I18" s="8">
         <v>225</v>
       </c>
-      <c r="J18" s="12">
+      <c r="J18" s="8">
         <v>215</v>
       </c>
-      <c r="K18" s="12">
+      <c r="K18" s="8">
         <v>174</v>
       </c>
-      <c r="L18" s="12">
+      <c r="L18" s="8">
         <v>162</v>
       </c>
-      <c r="M18" s="12">
+      <c r="M18" s="8">
         <v>214</v>
       </c>
-      <c r="N18" s="12">
+      <c r="N18" s="8">
         <v>142</v>
       </c>
-      <c r="O18" s="12">
+      <c r="O18" s="8">
         <v>254</v>
       </c>
-      <c r="P18" s="12">
+      <c r="P18" s="8">
         <v>275</v>
       </c>
-      <c r="Q18" s="12">
+      <c r="Q18" s="8">
         <v>268</v>
       </c>
-      <c r="R18" s="12">
+      <c r="R18" s="8">
         <v>187</v>
       </c>
     </row>
-    <row r="19" spans="2:18" s="12" customFormat="1" ht="8.25" x14ac:dyDescent="0.25">
-      <c r="B19" s="11" t="s">
+    <row r="19" spans="2:18" s="8" customFormat="1" ht="8.25" x14ac:dyDescent="0.25">
+      <c r="B19" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C19" s="12">
+      <c r="C19" s="8">
         <v>2944</v>
       </c>
-      <c r="D19" s="12">
+      <c r="D19" s="8">
         <v>2162</v>
       </c>
-      <c r="E19" s="12">
+      <c r="E19" s="8">
         <v>2020</v>
       </c>
-      <c r="F19" s="12">
+      <c r="F19" s="8">
         <v>2170</v>
       </c>
-      <c r="G19" s="12">
+      <c r="G19" s="8">
         <v>1892</v>
       </c>
-      <c r="H19" s="12">
+      <c r="H19" s="8">
         <v>2010</v>
       </c>
-      <c r="I19" s="12">
+      <c r="I19" s="8">
         <v>2361</v>
       </c>
-      <c r="J19" s="12">
+      <c r="J19" s="8">
         <v>1864</v>
       </c>
-      <c r="K19" s="12">
+      <c r="K19" s="8">
         <v>1657</v>
       </c>
-      <c r="L19" s="12">
+      <c r="L19" s="8">
         <v>1709</v>
       </c>
-      <c r="M19" s="12">
+      <c r="M19" s="8">
         <v>1278</v>
       </c>
-      <c r="N19" s="12">
+      <c r="N19" s="8">
         <v>1208</v>
       </c>
-      <c r="O19" s="12">
+      <c r="O19" s="8">
         <v>1185</v>
       </c>
-      <c r="P19" s="12">
+      <c r="P19" s="8">
         <v>1331</v>
       </c>
-      <c r="Q19" s="12">
+      <c r="Q19" s="8">
         <v>783</v>
       </c>
-      <c r="R19" s="12">
+      <c r="R19" s="8">
         <v>899</v>
       </c>
     </row>
-    <row r="20" spans="2:18" s="12" customFormat="1" ht="9" x14ac:dyDescent="0.25">
-      <c r="B20" s="11" t="s">
+    <row r="20" spans="2:18" s="8" customFormat="1" ht="9" x14ac:dyDescent="0.25">
+      <c r="B20" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C20" s="12">
+      <c r="C20" s="8">
         <v>41</v>
       </c>
-      <c r="D20" s="12">
+      <c r="D20" s="8">
         <v>36</v>
       </c>
-      <c r="E20" s="12">
+      <c r="E20" s="8">
         <v>39</v>
       </c>
-      <c r="F20" s="12">
+      <c r="F20" s="8">
         <v>24</v>
       </c>
-      <c r="G20" s="12">
+      <c r="G20" s="8">
         <v>21</v>
       </c>
-      <c r="H20" s="12">
+      <c r="H20" s="8">
         <v>28</v>
       </c>
-      <c r="I20" s="12">
+      <c r="I20" s="8">
         <v>20</v>
       </c>
-      <c r="J20" s="12">
+      <c r="J20" s="8">
         <v>55</v>
       </c>
-      <c r="K20" s="12">
+      <c r="K20" s="8">
         <v>64</v>
       </c>
-      <c r="L20" s="12">
+      <c r="L20" s="8">
         <v>63</v>
       </c>
-      <c r="M20" s="12">
+      <c r="M20" s="8">
         <v>295</v>
       </c>
-      <c r="N20" s="12">
+      <c r="N20" s="8">
         <v>672</v>
       </c>
-      <c r="O20" s="12">
+      <c r="O20" s="8">
         <v>582</v>
       </c>
-      <c r="P20" s="12">
+      <c r="P20" s="8">
         <v>2217</v>
       </c>
-      <c r="Q20" s="12">
+      <c r="Q20" s="8">
         <v>441</v>
       </c>
-      <c r="R20" s="12">
+      <c r="R20" s="8">
         <v>150</v>
       </c>
     </row>
-    <row r="21" spans="2:18" s="12" customFormat="1" ht="9" x14ac:dyDescent="0.25">
-      <c r="B21" s="11" t="s">
+    <row r="21" spans="2:18" s="8" customFormat="1" ht="9" x14ac:dyDescent="0.25">
+      <c r="B21" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C21" s="12">
+      <c r="C21" s="8">
         <v>1534</v>
       </c>
-      <c r="D21" s="12">
+      <c r="D21" s="8">
         <v>1289</v>
       </c>
-      <c r="E21" s="12">
+      <c r="E21" s="8">
         <v>1232</v>
       </c>
-      <c r="F21" s="12">
+      <c r="F21" s="8">
         <v>1017</v>
       </c>
-      <c r="G21" s="12">
+      <c r="G21" s="8">
         <v>1165</v>
       </c>
-      <c r="H21" s="12">
+      <c r="H21" s="8">
         <v>1263</v>
       </c>
-      <c r="I21" s="12">
+      <c r="I21" s="8">
         <v>1482</v>
       </c>
-      <c r="J21" s="12">
+      <c r="J21" s="8">
         <v>1739</v>
       </c>
-      <c r="K21" s="12">
+      <c r="K21" s="8">
         <v>1769</v>
       </c>
-      <c r="L21" s="12">
+      <c r="L21" s="8">
         <v>1765</v>
       </c>
-      <c r="M21" s="12">
+      <c r="M21" s="8">
         <v>2262</v>
       </c>
-      <c r="N21" s="12">
+      <c r="N21" s="8">
         <v>2787</v>
       </c>
-      <c r="O21" s="12">
+      <c r="O21" s="8">
         <v>2501</v>
       </c>
-      <c r="P21" s="12">
+      <c r="P21" s="8">
         <v>4241</v>
       </c>
-      <c r="Q21" s="12">
+      <c r="Q21" s="8">
         <v>2376</v>
       </c>
-      <c r="R21" s="12">
+      <c r="R21" s="8">
         <v>2243</v>
       </c>
     </row>
-    <row r="22" spans="2:18" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25">
-      <c r="B22" s="9" t="s">
+    <row r="22" spans="2:18" s="6" customFormat="1" ht="8.25" x14ac:dyDescent="0.25">
+      <c r="B22" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C22" s="10">
+      <c r="C22" s="6">
         <v>525</v>
       </c>
-      <c r="D22" s="10">
+      <c r="D22" s="6">
         <v>521</v>
       </c>
-      <c r="E22" s="10">
+      <c r="E22" s="6">
         <v>564</v>
       </c>
-      <c r="F22" s="10">
+      <c r="F22" s="6">
         <v>542</v>
       </c>
-      <c r="G22" s="10">
+      <c r="G22" s="6">
         <v>489</v>
       </c>
-      <c r="H22" s="10">
+      <c r="H22" s="6">
         <v>599</v>
       </c>
-      <c r="I22" s="10">
+      <c r="I22" s="6">
         <v>596</v>
       </c>
-      <c r="J22" s="10">
+      <c r="J22" s="6">
         <v>589</v>
       </c>
-      <c r="K22" s="10">
+      <c r="K22" s="6">
         <v>596</v>
       </c>
-      <c r="L22" s="10">
+      <c r="L22" s="6">
         <v>625</v>
       </c>
-      <c r="M22" s="10">
+      <c r="M22" s="6">
         <v>647</v>
       </c>
-      <c r="N22" s="10">
+      <c r="N22" s="6">
         <v>673</v>
       </c>
-      <c r="O22" s="10">
+      <c r="O22" s="6">
         <v>658</v>
       </c>
-      <c r="P22" s="10">
+      <c r="P22" s="6">
         <v>661</v>
       </c>
-      <c r="Q22" s="10">
+      <c r="Q22" s="6">
         <v>744</v>
       </c>
-      <c r="R22" s="10">
+      <c r="R22" s="6">
         <v>793</v>
       </c>
     </row>
-    <row r="23" spans="2:18" s="12" customFormat="1" ht="8.25" x14ac:dyDescent="0.25">
-      <c r="B23" s="11" t="s">
+    <row r="23" spans="2:18" s="8" customFormat="1" ht="8.25" x14ac:dyDescent="0.25">
+      <c r="B23" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C23" s="12">
+      <c r="C23" s="8">
         <v>81</v>
       </c>
-      <c r="D23" s="12">
+      <c r="D23" s="8">
         <v>112</v>
       </c>
-      <c r="E23" s="12">
+      <c r="E23" s="8">
         <v>76</v>
       </c>
-      <c r="F23" s="12">
+      <c r="F23" s="8">
         <v>73</v>
       </c>
-      <c r="G23" s="12">
+      <c r="G23" s="8">
         <v>89</v>
       </c>
-      <c r="H23" s="12">
+      <c r="H23" s="8">
         <v>96</v>
       </c>
-      <c r="I23" s="12">
+      <c r="I23" s="8">
         <v>110</v>
       </c>
-      <c r="J23" s="12">
+      <c r="J23" s="8">
         <v>111</v>
       </c>
-      <c r="K23" s="12">
+      <c r="K23" s="8">
         <v>119</v>
       </c>
-      <c r="L23" s="12">
+      <c r="L23" s="8">
         <v>112</v>
       </c>
-      <c r="M23" s="12">
+      <c r="M23" s="8">
         <v>134</v>
       </c>
-      <c r="N23" s="12">
+      <c r="N23" s="8">
         <v>108</v>
       </c>
-      <c r="O23" s="12">
+      <c r="O23" s="8">
         <v>119</v>
       </c>
-      <c r="P23" s="12">
+      <c r="P23" s="8">
         <v>124</v>
       </c>
-      <c r="Q23" s="12">
+      <c r="Q23" s="8">
         <v>150</v>
       </c>
-      <c r="R23" s="12">
+      <c r="R23" s="8">
         <v>142</v>
       </c>
     </row>
-    <row r="24" spans="2:18" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25">
-      <c r="B24" s="9" t="s">
+    <row r="24" spans="2:18" s="6" customFormat="1" ht="8.25" x14ac:dyDescent="0.25">
+      <c r="B24" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C24" s="10">
+      <c r="C24" s="6">
         <v>250</v>
       </c>
-      <c r="D24" s="10">
+      <c r="D24" s="6">
         <v>266</v>
       </c>
-      <c r="E24" s="10">
+      <c r="E24" s="6">
         <v>233</v>
       </c>
-      <c r="F24" s="10">
+      <c r="F24" s="6">
         <v>211</v>
       </c>
-      <c r="G24" s="10">
+      <c r="G24" s="6">
         <v>225</v>
       </c>
-      <c r="H24" s="10">
+      <c r="H24" s="6">
         <v>211</v>
       </c>
-      <c r="I24" s="10">
+      <c r="I24" s="6">
         <v>211</v>
       </c>
-      <c r="J24" s="10">
+      <c r="J24" s="6">
         <v>228</v>
       </c>
-      <c r="K24" s="10">
+      <c r="K24" s="6">
         <v>256</v>
       </c>
-      <c r="L24" s="10">
+      <c r="L24" s="6">
         <v>260</v>
       </c>
-      <c r="M24" s="10">
+      <c r="M24" s="6">
         <v>270</v>
       </c>
-      <c r="N24" s="10">
+      <c r="N24" s="6">
         <v>296</v>
       </c>
-      <c r="O24" s="10">
+      <c r="O24" s="6">
         <v>247</v>
       </c>
-      <c r="P24" s="10">
+      <c r="P24" s="6">
         <v>288</v>
       </c>
-      <c r="Q24" s="10">
+      <c r="Q24" s="6">
         <v>272</v>
       </c>
-      <c r="R24" s="10">
+      <c r="R24" s="6">
         <v>293</v>
       </c>
     </row>
-    <row r="25" spans="2:18" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25">
-      <c r="B25" s="9" t="s">
+    <row r="25" spans="2:18" s="6" customFormat="1" ht="8.25" x14ac:dyDescent="0.25">
+      <c r="B25" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C25" s="10">
+      <c r="C25" s="6">
         <v>2851</v>
       </c>
-      <c r="D25" s="10">
+      <c r="D25" s="6">
         <v>2375</v>
       </c>
-      <c r="E25" s="10">
+      <c r="E25" s="6">
         <v>2272</v>
       </c>
-      <c r="F25" s="10">
+      <c r="F25" s="6">
         <v>2338</v>
       </c>
-      <c r="G25" s="10">
+      <c r="G25" s="6">
         <v>2290</v>
       </c>
-      <c r="H25" s="10">
+      <c r="H25" s="6">
         <v>2443</v>
       </c>
-      <c r="I25" s="10">
+      <c r="I25" s="6">
         <v>2488</v>
       </c>
-      <c r="J25" s="10">
+      <c r="J25" s="6">
         <v>2348</v>
       </c>
-      <c r="K25" s="10">
+      <c r="K25" s="6">
         <v>2364</v>
       </c>
-      <c r="L25" s="10">
+      <c r="L25" s="6">
         <v>2392</v>
       </c>
-      <c r="M25" s="10">
+      <c r="M25" s="6">
         <v>2614</v>
       </c>
-      <c r="N25" s="10">
+      <c r="N25" s="6">
         <v>2599</v>
       </c>
-      <c r="O25" s="10">
+      <c r="O25" s="6">
         <v>2694</v>
       </c>
-      <c r="P25" s="10">
+      <c r="P25" s="6">
         <v>3120</v>
       </c>
-      <c r="Q25" s="10">
+      <c r="Q25" s="6">
         <v>3645</v>
       </c>
-      <c r="R25" s="10">
+      <c r="R25" s="6">
         <v>5045</v>
       </c>
     </row>
-    <row r="26" spans="2:18" s="12" customFormat="1" ht="8.25" x14ac:dyDescent="0.25">
-      <c r="B26" s="11" t="s">
+    <row r="26" spans="2:18" s="8" customFormat="1" ht="8.25" x14ac:dyDescent="0.25">
+      <c r="B26" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C26" s="12">
+      <c r="C26" s="8">
         <v>227</v>
       </c>
-      <c r="D26" s="12">
+      <c r="D26" s="8">
         <v>230</v>
       </c>
-      <c r="E26" s="12">
+      <c r="E26" s="8">
         <v>219</v>
       </c>
-      <c r="F26" s="12">
+      <c r="F26" s="8">
         <v>210</v>
       </c>
-      <c r="G26" s="12">
+      <c r="G26" s="8">
         <v>161</v>
       </c>
-      <c r="H26" s="12">
+      <c r="H26" s="8">
         <v>124</v>
       </c>
-      <c r="I26" s="12">
+      <c r="I26" s="8">
         <v>121</v>
       </c>
-      <c r="J26" s="12">
+      <c r="J26" s="8">
         <v>129</v>
       </c>
-      <c r="K26" s="12">
+      <c r="K26" s="8">
         <v>129</v>
       </c>
-      <c r="L26" s="12">
+      <c r="L26" s="8">
         <v>129</v>
       </c>
-      <c r="M26" s="12">
+      <c r="M26" s="8">
         <v>150</v>
       </c>
-      <c r="N26" s="12">
+      <c r="N26" s="8">
         <v>158</v>
       </c>
-      <c r="O26" s="12">
+      <c r="O26" s="8">
         <v>131</v>
       </c>
-      <c r="P26" s="12">
+      <c r="P26" s="8">
         <v>167</v>
       </c>
-      <c r="Q26" s="12">
+      <c r="Q26" s="8">
         <v>184</v>
       </c>
-      <c r="R26" s="12">
+      <c r="R26" s="8">
         <v>292</v>
       </c>
     </row>
-    <row r="27" spans="2:18" s="12" customFormat="1" ht="8.25" x14ac:dyDescent="0.25">
-      <c r="B27" s="11" t="s">
+    <row r="27" spans="2:18" s="8" customFormat="1" ht="8.25" x14ac:dyDescent="0.25">
+      <c r="B27" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C27" s="12">
+      <c r="C27" s="8">
         <v>454</v>
       </c>
-      <c r="D27" s="12">
+      <c r="D27" s="8">
         <v>377</v>
       </c>
-      <c r="E27" s="12">
+      <c r="E27" s="8">
         <v>367</v>
       </c>
-      <c r="F27" s="12">
+      <c r="F27" s="8">
         <v>335</v>
       </c>
-      <c r="G27" s="12">
+      <c r="G27" s="8">
         <v>295</v>
       </c>
-      <c r="H27" s="12">
+      <c r="H27" s="8">
         <v>240</v>
       </c>
-      <c r="I27" s="12">
+      <c r="I27" s="8">
         <v>209</v>
       </c>
-      <c r="J27" s="12">
+      <c r="J27" s="8">
         <v>243</v>
       </c>
-      <c r="K27" s="12">
+      <c r="K27" s="8">
         <v>254</v>
       </c>
-      <c r="L27" s="12">
+      <c r="L27" s="8">
         <v>259</v>
       </c>
-      <c r="M27" s="12">
+      <c r="M27" s="8">
         <v>303</v>
       </c>
-      <c r="N27" s="12">
+      <c r="N27" s="8">
         <v>238</v>
       </c>
-      <c r="O27" s="12">
+      <c r="O27" s="8">
         <v>233</v>
       </c>
-      <c r="P27" s="12">
+      <c r="P27" s="8">
         <v>209</v>
       </c>
-      <c r="Q27" s="12">
+      <c r="Q27" s="8">
         <v>194</v>
       </c>
-      <c r="R27" s="12">
+      <c r="R27" s="8">
         <v>200</v>
       </c>
     </row>
-    <row r="28" spans="2:18" s="12" customFormat="1" ht="8.25" x14ac:dyDescent="0.25">
-      <c r="B28" s="11" t="s">
+    <row r="28" spans="2:18" s="8" customFormat="1" ht="8.25" x14ac:dyDescent="0.25">
+      <c r="B28" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C28" s="12">
+      <c r="C28" s="8">
         <v>44</v>
       </c>
-      <c r="D28" s="12">
+      <c r="D28" s="8">
         <v>33</v>
       </c>
-      <c r="E28" s="12">
+      <c r="E28" s="8">
         <v>38</v>
       </c>
-      <c r="F28" s="12">
+      <c r="F28" s="8">
         <v>34</v>
       </c>
-      <c r="G28" s="12">
+      <c r="G28" s="8">
         <v>41</v>
       </c>
-      <c r="H28" s="12">
+      <c r="H28" s="8">
         <v>44</v>
       </c>
-      <c r="I28" s="12">
+      <c r="I28" s="8">
         <v>64</v>
       </c>
-      <c r="J28" s="12">
+      <c r="J28" s="8">
         <v>61</v>
       </c>
-      <c r="K28" s="12">
+      <c r="K28" s="8">
         <v>63</v>
       </c>
-      <c r="L28" s="12">
+      <c r="L28" s="8">
         <v>65</v>
       </c>
-      <c r="M28" s="12">
+      <c r="M28" s="8">
         <v>96</v>
       </c>
-      <c r="N28" s="12">
+      <c r="N28" s="8">
         <v>103</v>
       </c>
-      <c r="O28" s="12">
+      <c r="O28" s="8">
         <v>73</v>
       </c>
-      <c r="P28" s="12">
+      <c r="P28" s="8">
         <v>157</v>
       </c>
-      <c r="Q28" s="12">
+      <c r="Q28" s="8">
         <v>117</v>
       </c>
-      <c r="R28" s="12">
+      <c r="R28" s="8">
         <v>131</v>
       </c>
     </row>
-    <row r="29" spans="2:18" s="12" customFormat="1" ht="8.25" x14ac:dyDescent="0.25">
-      <c r="B29" s="11" t="s">
+    <row r="29" spans="2:18" s="8" customFormat="1" ht="8.25" x14ac:dyDescent="0.25">
+      <c r="B29" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C29" s="12">
+      <c r="C29" s="8">
         <v>251</v>
       </c>
-      <c r="D29" s="12">
+      <c r="D29" s="8">
         <v>286</v>
       </c>
-      <c r="E29" s="12">
+      <c r="E29" s="8">
         <v>306</v>
       </c>
-      <c r="F29" s="12">
+      <c r="F29" s="8">
         <v>361</v>
       </c>
-      <c r="G29" s="12">
+      <c r="G29" s="8">
         <v>392</v>
       </c>
-      <c r="H29" s="12">
+      <c r="H29" s="8">
         <v>434</v>
       </c>
-      <c r="I29" s="12">
+      <c r="I29" s="8">
         <v>273</v>
       </c>
-      <c r="J29" s="12">
+      <c r="J29" s="8">
         <v>326</v>
       </c>
-      <c r="K29" s="12">
+      <c r="K29" s="8">
         <v>317</v>
       </c>
-      <c r="L29" s="12">
+      <c r="L29" s="8">
         <v>313</v>
       </c>
-      <c r="M29" s="12">
+      <c r="M29" s="8">
         <v>430</v>
       </c>
-      <c r="N29" s="12">
+      <c r="N29" s="8">
         <v>403</v>
       </c>
-      <c r="O29" s="12">
+      <c r="O29" s="8">
         <v>389</v>
       </c>
-      <c r="P29" s="12">
+      <c r="P29" s="8">
         <v>465</v>
       </c>
-      <c r="Q29" s="12">
+      <c r="Q29" s="8">
         <v>477</v>
       </c>
-      <c r="R29" s="12">
+      <c r="R29" s="8">
         <v>527</v>
       </c>
     </row>
-    <row r="30" spans="2:18" s="12" customFormat="1" ht="8.25" x14ac:dyDescent="0.25">
-      <c r="B30" s="11" t="s">
+    <row r="30" spans="2:18" s="8" customFormat="1" ht="8.25" x14ac:dyDescent="0.25">
+      <c r="B30" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C30" s="12">
+      <c r="C30" s="8">
         <v>386</v>
       </c>
-      <c r="D30" s="12">
+      <c r="D30" s="8">
         <v>362</v>
       </c>
-      <c r="E30" s="12">
+      <c r="E30" s="8">
         <v>303</v>
       </c>
-      <c r="F30" s="12">
+      <c r="F30" s="8">
         <v>323</v>
       </c>
-      <c r="G30" s="12">
+      <c r="G30" s="8">
         <v>245</v>
       </c>
-      <c r="H30" s="12">
+      <c r="H30" s="8">
         <v>255</v>
       </c>
-      <c r="I30" s="12">
+      <c r="I30" s="8">
         <v>227</v>
       </c>
-      <c r="J30" s="12">
+      <c r="J30" s="8">
         <v>227</v>
       </c>
-      <c r="K30" s="12">
+      <c r="K30" s="8">
         <v>262</v>
       </c>
-      <c r="L30" s="12">
+      <c r="L30" s="8">
         <v>221</v>
       </c>
-      <c r="M30" s="12">
+      <c r="M30" s="8">
         <v>255</v>
       </c>
-      <c r="N30" s="12">
+      <c r="N30" s="8">
         <v>260</v>
       </c>
-      <c r="O30" s="12">
+      <c r="O30" s="8">
         <v>243</v>
       </c>
-      <c r="P30" s="12">
+      <c r="P30" s="8">
         <v>308</v>
       </c>
-      <c r="Q30" s="12">
+      <c r="Q30" s="8">
         <v>336</v>
       </c>
-      <c r="R30" s="12">
+      <c r="R30" s="8">
         <v>331</v>
       </c>
     </row>
-    <row r="31" spans="2:18" s="12" customFormat="1" ht="8.25" x14ac:dyDescent="0.25">
-      <c r="B31" s="11" t="s">
+    <row r="31" spans="2:18" s="8" customFormat="1" ht="8.25" x14ac:dyDescent="0.25">
+      <c r="B31" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C31" s="13" t="s">
+      <c r="C31" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="D31" s="13" t="s">
+      <c r="D31" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="E31" s="13" t="s">
+      <c r="E31" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="F31" s="13" t="s">
+      <c r="F31" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="G31" s="13" t="s">
+      <c r="G31" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="H31" s="13" t="s">
+      <c r="H31" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="I31" s="13" t="s">
+      <c r="I31" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="J31" s="12">
+      <c r="J31" s="8">
         <v>17</v>
       </c>
-      <c r="K31" s="12">
+      <c r="K31" s="8">
         <v>23</v>
       </c>
-      <c r="L31" s="12">
+      <c r="L31" s="8">
         <v>23</v>
       </c>
-      <c r="M31" s="12">
+      <c r="M31" s="8">
         <v>53</v>
       </c>
-      <c r="N31" s="12">
+      <c r="N31" s="8">
         <v>24</v>
       </c>
-      <c r="O31" s="12">
+      <c r="O31" s="8">
         <v>59</v>
       </c>
-      <c r="P31" s="12">
+      <c r="P31" s="8">
         <v>43</v>
       </c>
-      <c r="Q31" s="12">
+      <c r="Q31" s="8">
         <v>42</v>
       </c>
-      <c r="R31" s="12">
+      <c r="R31" s="8">
         <v>145</v>
       </c>
     </row>
-    <row r="32" spans="2:18" s="12" customFormat="1" ht="8.25" x14ac:dyDescent="0.25">
-      <c r="B32" s="11" t="s">
+    <row r="32" spans="2:18" s="8" customFormat="1" ht="8.25" x14ac:dyDescent="0.25">
+      <c r="B32" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C32" s="12">
+      <c r="C32" s="8">
         <v>183</v>
       </c>
-      <c r="D32" s="12">
+      <c r="D32" s="8">
         <v>210</v>
       </c>
-      <c r="E32" s="12">
+      <c r="E32" s="8">
         <v>208</v>
       </c>
-      <c r="F32" s="12">
+      <c r="F32" s="8">
         <v>225</v>
       </c>
-      <c r="G32" s="12">
+      <c r="G32" s="8">
         <v>219</v>
       </c>
-      <c r="H32" s="12">
+      <c r="H32" s="8">
         <v>219</v>
       </c>
-      <c r="I32" s="12">
+      <c r="I32" s="8">
         <v>208</v>
       </c>
-      <c r="J32" s="12">
+      <c r="J32" s="8">
         <v>247</v>
       </c>
-      <c r="K32" s="12">
+      <c r="K32" s="8">
         <v>300</v>
       </c>
-      <c r="L32" s="12">
+      <c r="L32" s="8">
         <v>398</v>
       </c>
-      <c r="M32" s="12">
+      <c r="M32" s="8">
         <v>368</v>
       </c>
-      <c r="N32" s="12">
+      <c r="N32" s="8">
         <v>444</v>
       </c>
-      <c r="O32" s="12">
+      <c r="O32" s="8">
         <v>664</v>
       </c>
-      <c r="P32" s="12">
+      <c r="P32" s="8">
         <v>857</v>
       </c>
-      <c r="Q32" s="12">
+      <c r="Q32" s="8">
         <v>1414</v>
       </c>
-      <c r="R32" s="12">
+      <c r="R32" s="8">
         <v>2592</v>
       </c>
     </row>
-    <row r="33" spans="2:18" s="12" customFormat="1" ht="8.25" x14ac:dyDescent="0.25">
-      <c r="B33" s="11" t="s">
+    <row r="33" spans="2:18" s="8" customFormat="1" ht="8.25" x14ac:dyDescent="0.25">
+      <c r="B33" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="C33" s="12">
+      <c r="C33" s="8">
         <v>160</v>
       </c>
-      <c r="D33" s="12">
+      <c r="D33" s="8">
         <v>158</v>
       </c>
-      <c r="E33" s="12">
+      <c r="E33" s="8">
         <v>110</v>
       </c>
-      <c r="F33" s="12">
+      <c r="F33" s="8">
         <v>227</v>
       </c>
-      <c r="G33" s="12">
+      <c r="G33" s="8">
         <v>280</v>
       </c>
-      <c r="H33" s="12">
+      <c r="H33" s="8">
         <v>419</v>
       </c>
-      <c r="I33" s="12">
+      <c r="I33" s="8">
         <v>667</v>
       </c>
-      <c r="J33" s="12">
+      <c r="J33" s="8">
         <v>387</v>
       </c>
-      <c r="K33" s="12">
+      <c r="K33" s="8">
         <v>277</v>
       </c>
-      <c r="L33" s="12">
+      <c r="L33" s="8">
         <v>266</v>
       </c>
-      <c r="M33" s="12">
+      <c r="M33" s="8">
         <v>265</v>
       </c>
-      <c r="N33" s="12">
+      <c r="N33" s="8">
         <v>259</v>
       </c>
-      <c r="O33" s="12">
+      <c r="O33" s="8">
         <v>290</v>
       </c>
-      <c r="P33" s="12">
+      <c r="P33" s="8">
         <v>224</v>
       </c>
-      <c r="Q33" s="12">
+      <c r="Q33" s="8">
         <v>199</v>
       </c>
-      <c r="R33" s="12">
+      <c r="R33" s="8">
         <v>166</v>
       </c>
     </row>
-    <row r="34" spans="2:18" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25">
-      <c r="B34" s="9" t="s">
+    <row r="34" spans="2:18" s="6" customFormat="1" ht="8.25" x14ac:dyDescent="0.25">
+      <c r="B34" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C34" s="10">
+      <c r="C34" s="6">
         <v>2</v>
       </c>
-      <c r="D34" s="10">
+      <c r="D34" s="6">
         <v>1</v>
       </c>
-      <c r="E34" s="10">
+      <c r="E34" s="6">
         <v>0</v>
       </c>
-      <c r="F34" s="10">
+      <c r="F34" s="6">
         <v>1</v>
       </c>
-      <c r="G34" s="10">
+      <c r="G34" s="6">
         <v>2</v>
       </c>
-      <c r="H34" s="10">
+      <c r="H34" s="6">
         <v>3</v>
       </c>
-      <c r="I34" s="10">
+      <c r="I34" s="6">
         <v>2</v>
       </c>
-      <c r="J34" s="10">
+      <c r="J34" s="6">
         <v>1</v>
       </c>
-      <c r="K34" s="10">
+      <c r="K34" s="6">
         <v>0</v>
       </c>
-      <c r="L34" s="10">
+      <c r="L34" s="6">
         <v>1</v>
       </c>
-      <c r="M34" s="10">
+      <c r="M34" s="6">
         <v>0</v>
       </c>
-      <c r="N34" s="10">
+      <c r="N34" s="6">
         <v>2</v>
       </c>
-      <c r="O34" s="10">
+      <c r="O34" s="6">
         <v>1</v>
       </c>
-      <c r="P34" s="10">
+      <c r="P34" s="6">
         <v>3</v>
       </c>
-      <c r="Q34" s="10">
+      <c r="Q34" s="6">
         <v>5</v>
       </c>
-      <c r="R34" s="10">
+      <c r="R34" s="6">
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="2:18" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25">
-      <c r="B35" s="9" t="s">
+    <row r="35" spans="2:18" s="6" customFormat="1" ht="8.25" x14ac:dyDescent="0.25">
+      <c r="B35" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C35" s="10">
+      <c r="C35" s="6">
         <v>246</v>
       </c>
-      <c r="D35" s="10">
+      <c r="D35" s="6">
         <v>222</v>
       </c>
-      <c r="E35" s="10">
+      <c r="E35" s="6">
         <v>147</v>
       </c>
-      <c r="F35" s="10">
+      <c r="F35" s="6">
         <v>184</v>
       </c>
-      <c r="G35" s="10">
+      <c r="G35" s="6">
         <v>152</v>
       </c>
-      <c r="H35" s="10">
+      <c r="H35" s="6">
         <v>144</v>
       </c>
-      <c r="I35" s="10">
+      <c r="I35" s="6">
         <v>133</v>
       </c>
-      <c r="J35" s="10">
+      <c r="J35" s="6">
         <v>150</v>
       </c>
-      <c r="K35" s="10">
+      <c r="K35" s="6">
         <v>107</v>
       </c>
-      <c r="L35" s="10">
+      <c r="L35" s="6">
         <v>112</v>
       </c>
-      <c r="M35" s="10">
+      <c r="M35" s="6">
         <v>108</v>
       </c>
-      <c r="N35" s="10">
+      <c r="N35" s="6">
         <v>171</v>
       </c>
-      <c r="O35" s="10">
+      <c r="O35" s="6">
         <v>127</v>
       </c>
-      <c r="P35" s="10">
+      <c r="P35" s="6">
         <v>137</v>
       </c>
-      <c r="Q35" s="10">
+      <c r="Q35" s="6">
         <v>171</v>
       </c>
-      <c r="R35" s="10">
+      <c r="R35" s="6">
         <v>217</v>
       </c>
     </row>
-    <row r="36" spans="2:18" s="12" customFormat="1" ht="8.25" x14ac:dyDescent="0.25">
-      <c r="B36" s="11" t="s">
+    <row r="36" spans="2:18" s="8" customFormat="1" ht="8.25" x14ac:dyDescent="0.25">
+      <c r="B36" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="C36" s="12">
+      <c r="C36" s="8">
         <v>171</v>
       </c>
-      <c r="D36" s="12">
+      <c r="D36" s="8">
         <v>136</v>
       </c>
-      <c r="E36" s="12">
+      <c r="E36" s="8">
         <v>99</v>
       </c>
-      <c r="F36" s="12">
+      <c r="F36" s="8">
         <v>125</v>
       </c>
-      <c r="G36" s="12">
+      <c r="G36" s="8">
         <v>125</v>
       </c>
-      <c r="H36" s="12">
+      <c r="H36" s="8">
         <v>99</v>
       </c>
-      <c r="I36" s="12">
+      <c r="I36" s="8">
         <v>117</v>
       </c>
-      <c r="J36" s="12">
+      <c r="J36" s="8">
         <v>113</v>
       </c>
-      <c r="K36" s="12">
+      <c r="K36" s="8">
         <v>83</v>
       </c>
-      <c r="L36" s="12">
+      <c r="L36" s="8">
         <v>80</v>
       </c>
-      <c r="M36" s="12">
+      <c r="M36" s="8">
         <v>70</v>
       </c>
-      <c r="N36" s="12">
+      <c r="N36" s="8">
         <v>138</v>
       </c>
-      <c r="O36" s="12">
+      <c r="O36" s="8">
         <v>104</v>
       </c>
-      <c r="P36" s="12">
+      <c r="P36" s="8">
         <v>115</v>
       </c>
-      <c r="Q36" s="12">
+      <c r="Q36" s="8">
         <v>146</v>
       </c>
-      <c r="R36" s="12">
+      <c r="R36" s="8">
         <v>144</v>
       </c>
     </row>
-    <row r="37" spans="2:18" s="16" customFormat="1" ht="8.25" x14ac:dyDescent="0.25">
-      <c r="B37" s="14" t="s">
+    <row r="37" spans="2:18" s="12" customFormat="1" ht="8.25" x14ac:dyDescent="0.25">
+      <c r="B37" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="C37" s="15">
+      <c r="C37" s="11">
         <v>11441</v>
       </c>
-      <c r="D37" s="15">
+      <c r="D37" s="11">
         <v>9251</v>
       </c>
-      <c r="E37" s="15">
+      <c r="E37" s="11">
         <v>7704</v>
       </c>
-      <c r="F37" s="15">
+      <c r="F37" s="11">
         <v>7223</v>
       </c>
-      <c r="G37" s="15">
+      <c r="G37" s="11">
         <v>7363</v>
       </c>
-      <c r="H37" s="15">
+      <c r="H37" s="11">
         <v>7995</v>
       </c>
-      <c r="I37" s="15">
+      <c r="I37" s="11">
         <v>8526</v>
       </c>
-      <c r="J37" s="15">
+      <c r="J37" s="11">
         <v>8216</v>
       </c>
-      <c r="K37" s="15">
+      <c r="K37" s="11">
         <v>7722</v>
       </c>
-      <c r="L37" s="15">
+      <c r="L37" s="11">
         <v>7988</v>
       </c>
-      <c r="M37" s="15">
+      <c r="M37" s="11">
         <v>8519</v>
       </c>
-      <c r="N37" s="15">
+      <c r="N37" s="11">
         <v>8785</v>
       </c>
-      <c r="O37" s="15">
+      <c r="O37" s="11">
         <v>8470</v>
       </c>
-      <c r="P37" s="15">
+      <c r="P37" s="11">
         <v>10932</v>
       </c>
-      <c r="Q37" s="15">
+      <c r="Q37" s="11">
         <v>8878</v>
       </c>
-      <c r="R37" s="15">
+      <c r="R37" s="11">
         <v>10419</v>
       </c>
     </row>
-    <row r="38" spans="2:18" s="19" customFormat="1" ht="12" x14ac:dyDescent="0.25">
-      <c r="B38" s="17"/>
-      <c r="C38" s="18"/>
-      <c r="D38" s="18"/>
-      <c r="E38" s="18"/>
-      <c r="F38" s="18"/>
-      <c r="G38" s="18"/>
-      <c r="H38" s="18"/>
-      <c r="I38" s="18"/>
-      <c r="J38" s="18"/>
-      <c r="K38" s="18"/>
-      <c r="L38" s="18"/>
-      <c r="M38" s="18"/>
-      <c r="N38" s="18"/>
-      <c r="O38" s="18"/>
-      <c r="P38" s="18"/>
-    </row>
-    <row r="39" spans="2:18" s="19" customFormat="1" ht="12" x14ac:dyDescent="0.25">
-      <c r="B39" s="20" t="s">
+    <row r="38" spans="2:18" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.25">
+      <c r="B38" s="13"/>
+      <c r="C38" s="14"/>
+      <c r="D38" s="14"/>
+      <c r="E38" s="14"/>
+      <c r="F38" s="14"/>
+      <c r="G38" s="14"/>
+      <c r="H38" s="14"/>
+      <c r="I38" s="14"/>
+      <c r="J38" s="14"/>
+      <c r="K38" s="14"/>
+      <c r="L38" s="14"/>
+      <c r="M38" s="14"/>
+      <c r="N38" s="14"/>
+      <c r="O38" s="14"/>
+      <c r="P38" s="14"/>
+    </row>
+    <row r="39" spans="2:18" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.25">
+      <c r="B39" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="C39" s="18"/>
-      <c r="D39" s="18"/>
-      <c r="E39" s="18"/>
-      <c r="F39" s="18"/>
-      <c r="G39" s="18"/>
-      <c r="H39" s="18"/>
-      <c r="I39" s="18"/>
-      <c r="J39" s="18"/>
-      <c r="K39" s="18"/>
-      <c r="L39" s="18"/>
-      <c r="M39" s="18"/>
-      <c r="N39" s="18"/>
-      <c r="O39" s="18"/>
-      <c r="P39" s="18"/>
-    </row>
-    <row r="40" spans="2:18" s="19" customFormat="1" ht="12" x14ac:dyDescent="0.25">
-      <c r="B40" s="21" t="s">
+      <c r="C39" s="14"/>
+      <c r="D39" s="14"/>
+      <c r="E39" s="14"/>
+      <c r="F39" s="14"/>
+      <c r="G39" s="14"/>
+      <c r="H39" s="14"/>
+      <c r="I39" s="14"/>
+      <c r="J39" s="14"/>
+      <c r="K39" s="14"/>
+      <c r="L39" s="14"/>
+      <c r="M39" s="14"/>
+      <c r="N39" s="14"/>
+      <c r="O39" s="14"/>
+      <c r="P39" s="14"/>
+    </row>
+    <row r="40" spans="2:18" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.25">
+      <c r="B40" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="C40" s="18"/>
-      <c r="D40" s="18"/>
-      <c r="E40" s="18"/>
-      <c r="F40" s="18"/>
-      <c r="G40" s="18"/>
-      <c r="H40" s="18"/>
-      <c r="I40" s="18"/>
-      <c r="J40" s="18"/>
-      <c r="K40" s="18"/>
-      <c r="L40" s="18"/>
-      <c r="M40" s="18"/>
-      <c r="N40" s="18"/>
-      <c r="O40" s="18"/>
-      <c r="P40" s="18"/>
-    </row>
-    <row r="41" spans="2:18" s="19" customFormat="1" ht="12" x14ac:dyDescent="0.25">
-      <c r="B41" s="21" t="s">
+      <c r="C40" s="14"/>
+      <c r="D40" s="14"/>
+      <c r="E40" s="14"/>
+      <c r="F40" s="14"/>
+      <c r="G40" s="14"/>
+      <c r="H40" s="14"/>
+      <c r="I40" s="14"/>
+      <c r="J40" s="14"/>
+      <c r="K40" s="14"/>
+      <c r="L40" s="14"/>
+      <c r="M40" s="14"/>
+      <c r="N40" s="14"/>
+      <c r="O40" s="14"/>
+      <c r="P40" s="14"/>
+    </row>
+    <row r="41" spans="2:18" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.25">
+      <c r="B41" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="C41" s="18"/>
-      <c r="D41" s="18"/>
-      <c r="E41" s="18"/>
-      <c r="F41" s="18"/>
-      <c r="G41" s="18"/>
-      <c r="H41" s="18"/>
-      <c r="I41" s="18"/>
-      <c r="J41" s="18"/>
-      <c r="K41" s="18"/>
-      <c r="L41" s="18"/>
-      <c r="M41" s="18"/>
-      <c r="N41" s="18"/>
-      <c r="O41" s="18"/>
-      <c r="P41" s="18"/>
-    </row>
-    <row r="42" spans="2:18" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="12"/>
-    </row>
-    <row r="43" spans="2:18" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="12" t="s">
+      <c r="C41" s="14"/>
+      <c r="D41" s="14"/>
+      <c r="E41" s="14"/>
+      <c r="F41" s="14"/>
+      <c r="G41" s="14"/>
+      <c r="H41" s="14"/>
+      <c r="I41" s="14"/>
+      <c r="J41" s="14"/>
+      <c r="K41" s="14"/>
+      <c r="L41" s="14"/>
+      <c r="M41" s="14"/>
+      <c r="N41" s="14"/>
+      <c r="O41" s="14"/>
+      <c r="P41" s="14"/>
+    </row>
+    <row r="42" spans="2:18" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B42" s="8"/>
+    </row>
+    <row r="43" spans="2:18" s="3" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B43" s="8" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="44" spans="2:18" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="12"/>
-    </row>
-    <row r="45" spans="2:18" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="12" t="s">
+    <row r="44" spans="2:18" s="3" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B44" s="8"/>
+    </row>
+    <row r="45" spans="2:18" s="3" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B45" s="8" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="46" spans="2:18" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="12" t="s">
+    <row r="46" spans="2:18" s="3" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B46" s="8" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="47" spans="2:18" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="12" t="s">
+    <row r="47" spans="2:18" s="3" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B47" s="8" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="48" spans="2:18" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="22" t="s">
+    <row r="48" spans="2:18" s="3" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B48" s="18" t="s">
         <v>39</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Deploying to gh-pages from  @ 3c97e47585f7c03660b04bbb083e63370bc37f22 🚀
</commit_message>
<xml_diff>
--- a/assets/excel/2022_2-3-4.xlsx
+++ b/assets/excel/2022_2-3-4.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Hannover\Dez15-Uebergreifende-Analysen\Projekte\Integrationsmonitoring\github\MT_Site\assets\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E3FD296-6A78-4DCD-BEA3-E624EE584862}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7CED1319-FC21-4CB5-8326-E7F58BD13114}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14010" xr2:uid="{2C0D3989-42FD-490A-A21B-E034F5A30F90}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="10410" xr2:uid="{2C0D3989-42FD-490A-A21B-E034F5A30F90}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -173,9 +173,6 @@
     <t>2) einschl. britisch abhängiger Gebiete</t>
   </si>
   <si>
-    <t>3) Europa ab 2021 ohne Großbritannien</t>
-  </si>
-  <si>
     <t>Quelle: Einbürgerungsstatistik</t>
   </si>
   <si>
@@ -192,6 +189,9 @@
   </si>
   <si>
     <t>x</t>
+  </si>
+  <si>
+    <t>3) EU-Staaten ab 2021 ohne Großbritannien</t>
   </si>
 </sst>
 </file>
@@ -734,7 +734,7 @@
   <sheetPr codeName="Tabelle1"/>
   <dimension ref="B1:R48"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1066,13 +1066,13 @@
         <v>8</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F14" s="8">
         <v>34</v>
@@ -1967,25 +1967,25 @@
         <v>25</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D31" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E31" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F31" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G31" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H31" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I31" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J31" s="8">
         <v>17</v>
@@ -2390,7 +2390,7 @@
     </row>
     <row r="41" spans="2:18" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.25">
       <c r="B41" s="17" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="C41" s="14"/>
       <c r="D41" s="14"/>
@@ -2412,7 +2412,7 @@
     </row>
     <row r="43" spans="2:18" s="3" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B43" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="44" spans="2:18" s="3" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2420,22 +2420,22 @@
     </row>
     <row r="45" spans="2:18" s="3" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B45" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="46" spans="2:18" s="3" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B46" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="47" spans="2:18" s="3" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="48" spans="2:18" s="3" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B48" s="18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>